<commit_message>
Added additional HUC12's within supplyshed and updated Excel tracker.
</commit_message>
<xml_diff>
--- a/doc/tracking_hydrowork.xlsx
+++ b/doc/tracking_hydrowork.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20336"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ISU\Project\PhD\data\repo\G2G_supplyshed\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ISU\PhD\GIS\G2G_supplyshed\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845F6839-37C5-45B2-BE3B-1E3D167E18FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670B9497-5176-4913-BF09-A845A99818E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22185" windowHeight="12000" xr2:uid="{C39EBF64-7E6C-46AF-9D79-6A233BCEB030}"/>
+    <workbookView xWindow="8220" yWindow="852" windowWidth="17280" windowHeight="8964" xr2:uid="{C39EBF64-7E6C-46AF-9D79-6A233BCEB030}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>HUC12</t>
   </si>
@@ -78,9 +89,6 @@
     <t>Bennett Creek</t>
   </si>
   <si>
-    <t>Area in Supplyshed (%)</t>
-  </si>
-  <si>
     <t>Calamus Creek</t>
   </si>
   <si>
@@ -94,16 +102,32 @@
   </si>
   <si>
     <t>Pine Creek</t>
+  </si>
+  <si>
+    <t>Sugar Creek</t>
+  </si>
+  <si>
+    <t>AreaAcres</t>
+  </si>
+  <si>
+    <t>ClipArea</t>
+  </si>
+  <si>
+    <t>Bennett Creek-Sugar Creek</t>
+  </si>
+  <si>
+    <t>PerInSupshed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="000000000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +137,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -137,15 +168,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -473,22 +508,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C805B287-ED18-4AEF-A035-6F63FFC8E2C9}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,149 +533,327 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>70801030301</v>
+        <v>70801030408</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3">
+        <v>10212.6</v>
+      </c>
+      <c r="D2">
+        <v>10212.61</v>
+      </c>
+      <c r="E2" s="4">
+        <v>100.00009791825784</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>70801030302</v>
+        <v>70802060502</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3">
+        <v>28979.32</v>
+      </c>
+      <c r="D3">
+        <v>28686.84</v>
+      </c>
+      <c r="E3" s="4">
+        <v>98.990728560918612</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>70801030303</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="3">
+        <v>35846.199999999997</v>
+      </c>
+      <c r="D4">
+        <v>35351.050000000003</v>
+      </c>
+      <c r="E4" s="4">
+        <v>98.618682036031728</v>
+      </c>
+      <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>70801030404</v>
+        <v>70801030409</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3">
+        <v>22009.5</v>
+      </c>
+      <c r="D5">
+        <v>19422.59</v>
+      </c>
+      <c r="E5" s="4">
+        <v>88.246393602762438</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>70801030405</v>
+        <v>70802060601</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3">
+        <v>23416.959999999999</v>
+      </c>
+      <c r="D6">
+        <v>20493.439999999999</v>
+      </c>
+      <c r="E6" s="4">
+        <v>87.515373472901686</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>70801030407</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3">
+        <v>24272.14</v>
+      </c>
+      <c r="D7">
+        <v>19294.689999999999</v>
+      </c>
+      <c r="E7" s="4">
+        <v>79.493155527283548</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>70802060501</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3">
+        <v>27884.38</v>
+      </c>
+      <c r="D8">
+        <v>20005.400000000001</v>
+      </c>
+      <c r="E8" s="4">
+        <v>71.74410906751379</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>70801030302</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3">
+        <v>11995.61</v>
+      </c>
+      <c r="D9">
+        <v>6748.2520000000004</v>
+      </c>
+      <c r="E9" s="4">
+        <v>56.256013658330005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>70801030301</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3">
+        <v>29423.32</v>
+      </c>
+      <c r="D10">
+        <v>15008.4</v>
+      </c>
+      <c r="E10" s="4">
+        <v>51.008519772751683</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>70802060603</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3">
+        <v>22980.59</v>
+      </c>
+      <c r="D11">
+        <v>9151.6959999999999</v>
+      </c>
+      <c r="E11" s="4">
+        <v>39.823590255950784</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>70801030406</v>
+      </c>
+      <c r="B12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>70801030406</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>70801030407</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>70801030408</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>70801030409</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>70802060501</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>70802060502</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="3">
+        <v>38020.83</v>
+      </c>
+      <c r="D12">
+        <v>9854.3850000000002</v>
+      </c>
+      <c r="E12" s="4">
+        <v>25.918384738050172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>70802060503</v>
       </c>
       <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3">
+        <v>11278.66</v>
+      </c>
+      <c r="D13">
+        <v>2023.365</v>
+      </c>
+      <c r="E13" s="4">
+        <v>17.939764120915076</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>70801030603</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3">
+        <v>37253.97</v>
+      </c>
+      <c r="D14">
+        <v>3117.1970000000001</v>
+      </c>
+      <c r="E14" s="4">
+        <v>8.3674223176751372</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>70801010602</v>
+      </c>
+      <c r="B15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>70802060601</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>70801030603</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="3">
+        <v>25411.72</v>
+      </c>
+      <c r="D15">
+        <v>675.13589999999999</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2.6567894656481341</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <v>70801010602</v>
+        <v>70802060602</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="C16" s="3">
+        <v>28249.13</v>
+      </c>
+      <c r="D16">
+        <v>667.91399999999999</v>
+      </c>
+      <c r="E16" s="4">
+        <v>2.3643701593641997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>70801030404</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="3">
+        <v>11116.82</v>
+      </c>
+      <c r="D17">
+        <v>214.79949999999999</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1.93220273423515</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>70801030405</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="3">
+        <v>25613.38</v>
+      </c>
+      <c r="D18">
+        <v>117.2971</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.45795244516733052</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G18">
+    <sortCondition descending="1" ref="E1:E18"/>
+  </sortState>
+  <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>

</xml_diff>

<commit_message>
added in Thomas's progress.
</commit_message>
<xml_diff>
--- a/doc/tracking_hydrowork.xlsx
+++ b/doc/tracking_hydrowork.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20336"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ISU\PhD\GIS\G2G_supplyshed\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnel\Documents\Project\G2G_supplyshed\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670B9497-5176-4913-BF09-A845A99818E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0ECC4C-B978-4DEA-B29B-DA43430FB62B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8220" yWindow="852" windowWidth="17280" windowHeight="8964" xr2:uid="{C39EBF64-7E6C-46AF-9D79-6A233BCEB030}"/>
+    <workbookView xWindow="8220" yWindow="855" windowWidth="17280" windowHeight="8970" xr2:uid="{C39EBF64-7E6C-46AF-9D79-6A233BCEB030}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>HUC12</t>
   </si>
@@ -117,6 +106,9 @@
   </si>
   <si>
     <t>PerInSupshed</t>
+  </si>
+  <si>
+    <t>Thomas Kosacz</t>
   </si>
 </sst>
 </file>
@@ -511,21 +503,21 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,7 +540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>70801030408</v>
       </c>
@@ -565,7 +557,7 @@
         <v>100.00009791825784</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>70802060502</v>
       </c>
@@ -582,7 +574,7 @@
         <v>98.990728560918612</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>70801030303</v>
       </c>
@@ -605,7 +597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>70801030409</v>
       </c>
@@ -622,7 +614,7 @@
         <v>88.246393602762438</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>70802060601</v>
       </c>
@@ -638,8 +630,14 @@
       <c r="E6" s="4">
         <v>87.515373472901686</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>70801030407</v>
       </c>
@@ -656,7 +654,7 @@
         <v>79.493155527283548</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>70802060501</v>
       </c>
@@ -673,7 +671,7 @@
         <v>71.74410906751379</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>70801030302</v>
       </c>
@@ -690,7 +688,7 @@
         <v>56.256013658330005</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>70801030301</v>
       </c>
@@ -713,7 +711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>70802060603</v>
       </c>
@@ -730,7 +728,7 @@
         <v>39.823590255950784</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>70801030406</v>
       </c>
@@ -747,7 +745,7 @@
         <v>25.918384738050172</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>70802060503</v>
       </c>
@@ -764,7 +762,7 @@
         <v>17.939764120915076</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>70801030603</v>
       </c>
@@ -781,7 +779,7 @@
         <v>8.3674223176751372</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>70801010602</v>
       </c>
@@ -798,7 +796,7 @@
         <v>2.6567894656481341</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>70802060602</v>
       </c>
@@ -815,7 +813,7 @@
         <v>2.3643701593641997</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>70801030404</v>
       </c>
@@ -832,7 +830,7 @@
         <v>1.93220273423515</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>70801030405</v>
       </c>
@@ -850,7 +848,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G18">
+  <sortState ref="A2:G18">
     <sortCondition descending="1" ref="E1:E18"/>
   </sortState>
   <conditionalFormatting sqref="F1:F1048576">

</xml_diff>